<commit_message>
Updated YPS Cash Flow.xlsx
</commit_message>
<xml_diff>
--- a/Business Plan Documents/YPS Cash Flow.xlsx
+++ b/Business Plan Documents/YPS Cash Flow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cash Flow (Year 1)" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -571,6 +571,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,9 +883,9 @@
   </sheetPr>
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -985,51 +988,51 @@
       </c>
       <c r="C7" s="33">
         <f>B45</f>
-        <v>904892</v>
+        <v>1229750</v>
       </c>
       <c r="D7" s="33">
         <f t="shared" ref="D7:N7" si="1">C45</f>
-        <v>829296.21</v>
+        <v>1115653.21</v>
       </c>
       <c r="E7" s="33">
         <f t="shared" si="1"/>
-        <v>900860.41999999993</v>
+        <v>1118716.42</v>
       </c>
       <c r="F7" s="33">
         <f t="shared" si="1"/>
-        <v>928664.62999999989</v>
+        <v>1083019.6299999999</v>
       </c>
       <c r="G7" s="33">
         <f t="shared" si="1"/>
-        <v>1071768.8399999999</v>
+        <v>1116123.8399999999</v>
       </c>
       <c r="H7" s="33">
         <f t="shared" si="1"/>
-        <v>1274938.0499999998</v>
+        <v>1201793.0499999998</v>
       </c>
       <c r="I7" s="33">
         <f t="shared" si="1"/>
-        <v>1920717.2599999998</v>
+        <v>1660072.2599999998</v>
       </c>
       <c r="J7" s="33">
         <f t="shared" si="1"/>
-        <v>2938996.4699999997</v>
+        <v>2387101.4699999997</v>
       </c>
       <c r="K7" s="33">
         <f t="shared" si="1"/>
-        <v>4420525.68</v>
+        <v>3464880.6799999997</v>
       </c>
       <c r="L7" s="33">
         <f t="shared" si="1"/>
-        <v>5384979.8899999997</v>
+        <v>4154334.8899999997</v>
       </c>
       <c r="M7" s="33">
         <f t="shared" si="1"/>
-        <v>7135634.0999999996</v>
+        <v>5444989.0999999996</v>
       </c>
       <c r="N7" s="33">
         <f t="shared" si="1"/>
-        <v>8886288.3100000005</v>
+        <v>6735643.3099999996</v>
       </c>
       <c r="O7" s="33"/>
     </row>
@@ -1078,44 +1081,44 @@
         <v>0</v>
       </c>
       <c r="C10" s="12">
-        <v>206050</v>
+        <v>161050</v>
       </c>
       <c r="D10" s="12">
-        <v>343210</v>
+        <v>268210</v>
       </c>
       <c r="E10" s="12">
-        <v>344450</v>
+        <v>269450</v>
       </c>
       <c r="F10" s="12">
-        <v>479750</v>
+        <v>374750</v>
       </c>
       <c r="G10" s="12">
-        <v>514815</v>
+        <v>402315</v>
       </c>
       <c r="H10" s="12">
-        <v>862425</v>
+        <v>674925</v>
       </c>
       <c r="I10" s="12">
-        <v>1237425</v>
+        <v>956175</v>
       </c>
       <c r="J10" s="12">
-        <v>1725675</v>
+        <v>1331925</v>
       </c>
       <c r="K10" s="12">
-        <v>1188600</v>
+        <v>918600</v>
       </c>
       <c r="L10" s="12">
-        <v>1969800</v>
+        <v>1519800</v>
       </c>
       <c r="M10" s="12">
-        <v>1969800</v>
+        <v>1519800</v>
       </c>
       <c r="N10" s="12">
-        <v>2748760</v>
+        <v>2118760</v>
       </c>
       <c r="O10" s="10">
         <f t="shared" ref="O10:O12" si="2">SUM(B10:N10)</f>
-        <v>13590760</v>
+        <v>10515760</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -1224,55 +1227,55 @@
       </c>
       <c r="C13" s="10">
         <f t="shared" ref="C13:O13" si="3">SUM(C10:C12)</f>
-        <v>206050</v>
+        <v>161050</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="3"/>
-        <v>343210</v>
+        <v>268210</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="3"/>
-        <v>344450</v>
+        <v>269450</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="3"/>
-        <v>479750</v>
+        <v>374750</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="3"/>
-        <v>514815</v>
+        <v>402315</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="3"/>
-        <v>862425</v>
+        <v>674925</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="3"/>
-        <v>1237425</v>
+        <v>956175</v>
       </c>
       <c r="J13" s="10">
         <f t="shared" si="3"/>
-        <v>1725675</v>
+        <v>1331925</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="3"/>
-        <v>1188600</v>
+        <v>918600</v>
       </c>
       <c r="L13" s="10">
         <f t="shared" si="3"/>
-        <v>1969800</v>
+        <v>1519800</v>
       </c>
       <c r="M13" s="10">
         <f t="shared" si="3"/>
-        <v>1969800</v>
+        <v>1519800</v>
       </c>
       <c r="N13" s="10">
         <f t="shared" si="3"/>
-        <v>2748760</v>
+        <v>2118760</v>
       </c>
       <c r="O13" s="10">
         <f t="shared" si="3"/>
-        <v>14390760</v>
+        <v>11315760</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -1285,55 +1288,55 @@
       </c>
       <c r="C14" s="14">
         <f t="shared" ref="C14:O14" si="4">(C7+C13)</f>
-        <v>1110942</v>
+        <v>1390800</v>
       </c>
       <c r="D14" s="14">
         <f t="shared" si="4"/>
-        <v>1172506.21</v>
+        <v>1383863.21</v>
       </c>
       <c r="E14" s="14">
         <f t="shared" si="4"/>
-        <v>1245310.42</v>
+        <v>1388166.42</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="4"/>
-        <v>1408414.63</v>
+        <v>1457769.63</v>
       </c>
       <c r="G14" s="14">
         <f t="shared" si="4"/>
-        <v>1586583.8399999999</v>
+        <v>1518438.8399999999</v>
       </c>
       <c r="H14" s="14">
         <f t="shared" si="4"/>
-        <v>2137363.0499999998</v>
+        <v>1876718.0499999998</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="4"/>
-        <v>3158142.26</v>
+        <v>2616247.2599999998</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="4"/>
-        <v>4664671.47</v>
+        <v>3719026.4699999997</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="4"/>
-        <v>5609125.6799999997</v>
+        <v>4383480.68</v>
       </c>
       <c r="L14" s="14">
         <f t="shared" si="4"/>
-        <v>7354779.8899999997</v>
+        <v>5674134.8899999997</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" si="4"/>
-        <v>9105434.0999999996</v>
+        <v>6964789.0999999996</v>
       </c>
       <c r="N14" s="14">
         <f t="shared" si="4"/>
-        <v>11635048.310000001</v>
+        <v>8854403.3099999987</v>
       </c>
       <c r="O14" s="14">
         <f t="shared" si="4"/>
-        <v>14390760</v>
+        <v>11315760</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1425,7 +1428,7 @@
         <v>42</v>
       </c>
       <c r="B18" s="10">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="C18" s="10">
         <v>5000</v>
@@ -1465,7 +1468,7 @@
       </c>
       <c r="O18" s="10">
         <f>SUM(B18:N18)</f>
-        <v>190000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -1473,7 +1476,7 @@
         <v>43</v>
       </c>
       <c r="B19" s="10">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="C19" s="10">
         <v>2500</v>
@@ -1513,7 +1516,7 @@
       </c>
       <c r="O19" s="10">
         <f>SUM(B19:N19)</f>
-        <v>95000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
@@ -1713,43 +1716,43 @@
         <v>13</v>
       </c>
       <c r="B24" s="10">
-        <v>80000</v>
+        <v>10000</v>
       </c>
       <c r="C24" s="10">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D24" s="10">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="E24" s="10">
         <v>5000</v>
       </c>
       <c r="F24" s="10">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="G24" s="10">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H24" s="10">
         <v>5000</v>
       </c>
       <c r="I24" s="10">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J24" s="10">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="K24" s="10">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="L24" s="10">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M24" s="10">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="N24" s="10">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="O24" s="10">
         <f t="shared" si="5"/>
@@ -1908,13 +1911,13 @@
         <v>24000</v>
       </c>
       <c r="C28" s="10">
-        <v>7999</v>
+        <v>0</v>
       </c>
       <c r="D28" s="10">
-        <v>7999</v>
+        <v>0</v>
       </c>
       <c r="E28" s="10">
-        <v>7999</v>
+        <v>0</v>
       </c>
       <c r="F28" s="10">
         <v>7999</v>
@@ -1945,7 +1948,7 @@
       </c>
       <c r="O28" s="10">
         <f t="shared" si="5"/>
-        <v>119988</v>
+        <v>95991</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -2004,13 +2007,13 @@
         <v>10500</v>
       </c>
       <c r="C30" s="10">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="E30" s="10">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="F30" s="10">
         <v>3500</v>
@@ -2041,7 +2044,7 @@
       </c>
       <c r="O30" s="10">
         <f t="shared" si="5"/>
-        <v>52500</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -2193,7 +2196,7 @@
         <v>44</v>
       </c>
       <c r="B34" s="10">
-        <v>160000</v>
+        <v>40000</v>
       </c>
       <c r="C34" s="10">
         <v>10000</v>
@@ -2233,7 +2236,7 @@
       </c>
       <c r="O34" s="10">
         <f t="shared" si="5"/>
-        <v>280000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
@@ -2241,7 +2244,7 @@
         <v>45</v>
       </c>
       <c r="B35" s="10">
-        <v>1108</v>
+        <v>1250</v>
       </c>
       <c r="C35" s="10">
         <v>0</v>
@@ -2281,7 +2284,7 @@
       </c>
       <c r="O35" s="10">
         <f t="shared" si="5"/>
-        <v>1108</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -2386,27 +2389,27 @@
       </c>
       <c r="B38" s="10">
         <f>SUM(B17:B37)</f>
-        <v>495108</v>
+        <v>170250</v>
       </c>
       <c r="C38" s="10">
         <f t="shared" ref="C38:O38" si="6">SUM(C17:C37)</f>
-        <v>245098</v>
+        <v>238599</v>
       </c>
       <c r="D38" s="10">
         <f t="shared" si="6"/>
-        <v>235098</v>
+        <v>228599</v>
       </c>
       <c r="E38" s="10">
         <f t="shared" si="6"/>
-        <v>280098</v>
+        <v>268599</v>
       </c>
       <c r="F38" s="10">
         <f t="shared" si="6"/>
-        <v>300098</v>
+        <v>305098</v>
       </c>
       <c r="G38" s="10">
         <f t="shared" si="6"/>
-        <v>275098</v>
+        <v>280098</v>
       </c>
       <c r="H38" s="10">
         <f t="shared" si="6"/>
@@ -2414,31 +2417,31 @@
       </c>
       <c r="I38" s="10">
         <f t="shared" si="6"/>
-        <v>182598</v>
+        <v>192598</v>
       </c>
       <c r="J38" s="10">
         <f t="shared" si="6"/>
-        <v>207598</v>
+        <v>217598</v>
       </c>
       <c r="K38" s="10">
         <f t="shared" si="6"/>
-        <v>187598</v>
+        <v>192598</v>
       </c>
       <c r="L38" s="10">
         <f t="shared" si="6"/>
-        <v>182598</v>
+        <v>192598</v>
       </c>
       <c r="M38" s="10">
         <f t="shared" si="6"/>
-        <v>182598</v>
+        <v>192598</v>
       </c>
       <c r="N38" s="10">
         <f t="shared" si="6"/>
-        <v>212598</v>
+        <v>217598</v>
       </c>
       <c r="O38" s="10">
         <f t="shared" si="6"/>
-        <v>3166284</v>
+        <v>2876929</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -2687,27 +2690,27 @@
       </c>
       <c r="B44" s="10">
         <f>SUM(B38:B43)</f>
-        <v>495108</v>
+        <v>170250</v>
       </c>
       <c r="C44" s="10">
         <f t="shared" ref="C44:O44" si="7">SUM(C38:C43)</f>
-        <v>281645.78999999998</v>
+        <v>275146.78999999998</v>
       </c>
       <c r="D44" s="10">
         <f t="shared" si="7"/>
-        <v>271645.78999999998</v>
+        <v>265146.78999999998</v>
       </c>
       <c r="E44" s="10">
         <f t="shared" si="7"/>
-        <v>316645.78999999998</v>
+        <v>305146.78999999998</v>
       </c>
       <c r="F44" s="10">
         <f t="shared" si="7"/>
-        <v>336645.79</v>
+        <v>341645.79</v>
       </c>
       <c r="G44" s="10">
         <f t="shared" si="7"/>
-        <v>311645.78999999998</v>
+        <v>316645.78999999998</v>
       </c>
       <c r="H44" s="10">
         <f t="shared" si="7"/>
@@ -2715,31 +2718,31 @@
       </c>
       <c r="I44" s="10">
         <f t="shared" si="7"/>
-        <v>219145.79</v>
+        <v>229145.79</v>
       </c>
       <c r="J44" s="10">
         <f t="shared" si="7"/>
-        <v>244145.79</v>
+        <v>254145.79</v>
       </c>
       <c r="K44" s="10">
         <f t="shared" si="7"/>
-        <v>224145.79</v>
+        <v>229145.79</v>
       </c>
       <c r="L44" s="10">
         <f t="shared" si="7"/>
-        <v>219145.79</v>
+        <v>229145.79</v>
       </c>
       <c r="M44" s="10">
         <f t="shared" si="7"/>
-        <v>219145.79</v>
+        <v>229145.79</v>
       </c>
       <c r="N44" s="10">
         <f t="shared" si="7"/>
-        <v>249145.79</v>
+        <v>254145.79</v>
       </c>
       <c r="O44" s="10">
         <f t="shared" si="7"/>
-        <v>3604857.48</v>
+        <v>3315502.48</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
@@ -2748,59 +2751,59 @@
       </c>
       <c r="B45" s="14">
         <f t="shared" ref="B45:O45" si="8">(B14-B44)</f>
-        <v>904892</v>
+        <v>1229750</v>
       </c>
       <c r="C45" s="14">
         <f t="shared" si="8"/>
-        <v>829296.21</v>
+        <v>1115653.21</v>
       </c>
       <c r="D45" s="14">
         <f t="shared" si="8"/>
-        <v>900860.41999999993</v>
+        <v>1118716.42</v>
       </c>
       <c r="E45" s="14">
         <f t="shared" si="8"/>
-        <v>928664.62999999989</v>
+        <v>1083019.6299999999</v>
       </c>
       <c r="F45" s="14">
         <f t="shared" si="8"/>
-        <v>1071768.8399999999</v>
+        <v>1116123.8399999999</v>
       </c>
       <c r="G45" s="14">
         <f t="shared" si="8"/>
-        <v>1274938.0499999998</v>
+        <v>1201793.0499999998</v>
       </c>
       <c r="H45" s="14">
         <f t="shared" si="8"/>
-        <v>1920717.2599999998</v>
+        <v>1660072.2599999998</v>
       </c>
       <c r="I45" s="14">
         <f t="shared" si="8"/>
-        <v>2938996.4699999997</v>
+        <v>2387101.4699999997</v>
       </c>
       <c r="J45" s="14">
         <f t="shared" si="8"/>
-        <v>4420525.68</v>
+        <v>3464880.6799999997</v>
       </c>
       <c r="K45" s="14">
         <f t="shared" si="8"/>
-        <v>5384979.8899999997</v>
+        <v>4154334.8899999997</v>
       </c>
       <c r="L45" s="14">
         <f t="shared" si="8"/>
-        <v>7135634.0999999996</v>
+        <v>5444989.0999999996</v>
       </c>
       <c r="M45" s="14">
         <f t="shared" si="8"/>
-        <v>8886288.3100000005</v>
+        <v>6735643.3099999996</v>
       </c>
       <c r="N45" s="14">
         <f t="shared" si="8"/>
-        <v>11385902.520000001</v>
+        <v>8600257.5199999996</v>
       </c>
       <c r="O45" s="14">
         <f t="shared" si="8"/>
-        <v>10785902.52</v>
+        <v>8000257.5199999996</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2966,14 +2969,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
-    <col min="2" max="15" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="15" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
@@ -3066,55 +3071,55 @@
         <v>2</v>
       </c>
       <c r="B7" s="14">
-        <v>11385903</v>
+        <v>8600258</v>
       </c>
       <c r="C7" s="33">
         <f>B45</f>
-        <v>11385903</v>
+        <v>8600258</v>
       </c>
       <c r="D7" s="33">
         <f t="shared" ref="D7:N7" si="1">C45</f>
-        <v>11982897.210000001</v>
+        <v>9017252.2100000009</v>
       </c>
       <c r="E7" s="33">
         <f t="shared" si="1"/>
-        <v>13014711.420000002</v>
+        <v>9773066.4200000018</v>
       </c>
       <c r="F7" s="33">
         <f t="shared" si="1"/>
-        <v>14264245.630000003</v>
+        <v>10698600.630000003</v>
       </c>
       <c r="G7" s="33">
         <f t="shared" si="1"/>
-        <v>15916739.840000004</v>
+        <v>11931094.840000004</v>
       </c>
       <c r="H7" s="33">
         <f t="shared" si="1"/>
-        <v>16721024.050000004</v>
+        <v>12510379.050000004</v>
       </c>
       <c r="I7" s="33">
         <f t="shared" si="1"/>
-        <v>18212168.260000005</v>
+        <v>13626523.260000005</v>
       </c>
       <c r="J7" s="33">
         <f t="shared" si="1"/>
-        <v>20453312.470000006</v>
+        <v>15305167.470000006</v>
       </c>
       <c r="K7" s="33">
         <f t="shared" si="1"/>
-        <v>23640956.680000007</v>
+        <v>17705311.680000007</v>
       </c>
       <c r="L7" s="33">
         <f t="shared" si="1"/>
-        <v>25198550.890000008</v>
+        <v>18857905.890000008</v>
       </c>
       <c r="M7" s="33">
         <f t="shared" si="1"/>
-        <v>27927945.100000009</v>
+        <v>20912300.100000009</v>
       </c>
       <c r="N7" s="33">
         <f t="shared" si="1"/>
-        <v>30657339.31000001</v>
+        <v>22966694.31000001</v>
       </c>
       <c r="O7" s="33"/>
     </row>
@@ -3162,45 +3167,45 @@
       <c r="B10" s="12">
         <v>0</v>
       </c>
-      <c r="C10" s="12">
-        <v>816140</v>
-      </c>
-      <c r="D10" s="12">
-        <v>1250960</v>
-      </c>
-      <c r="E10" s="12">
-        <v>1468680</v>
-      </c>
-      <c r="F10" s="12">
-        <v>1901640</v>
-      </c>
-      <c r="G10" s="12">
-        <v>1023430</v>
-      </c>
-      <c r="H10" s="12">
-        <v>1710290</v>
-      </c>
-      <c r="I10" s="12">
-        <v>2460290</v>
-      </c>
-      <c r="J10" s="12">
-        <v>3436790</v>
-      </c>
-      <c r="K10" s="12">
-        <v>1776740</v>
-      </c>
-      <c r="L10" s="12">
-        <v>2948540</v>
-      </c>
-      <c r="M10" s="12">
-        <v>2948540</v>
-      </c>
-      <c r="N10" s="12">
-        <v>4118100</v>
+      <c r="C10" s="40">
+        <v>636140</v>
+      </c>
+      <c r="D10" s="40">
+        <v>974960</v>
+      </c>
+      <c r="E10" s="40">
+        <v>1144680</v>
+      </c>
+      <c r="F10" s="40">
+        <v>1481640</v>
+      </c>
+      <c r="G10" s="40">
+        <v>798430</v>
+      </c>
+      <c r="H10" s="40">
+        <v>1335290</v>
+      </c>
+      <c r="I10" s="40">
+        <v>1897790</v>
+      </c>
+      <c r="J10" s="40">
+        <v>2649290</v>
+      </c>
+      <c r="K10" s="40">
+        <v>1371740</v>
+      </c>
+      <c r="L10" s="40">
+        <v>2273540</v>
+      </c>
+      <c r="M10" s="40">
+        <v>2273540</v>
+      </c>
+      <c r="N10" s="40">
+        <v>3173100</v>
       </c>
       <c r="O10" s="12">
         <f>SUM(C10:N10)</f>
-        <v>25860140</v>
+        <v>20010140</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -3309,55 +3314,55 @@
       </c>
       <c r="C13" s="10">
         <f t="shared" ref="C13:O13" si="2">SUM(C10:C12)</f>
-        <v>816140</v>
+        <v>636140</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="2"/>
-        <v>1250960</v>
+        <v>974960</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="2"/>
-        <v>1468680</v>
+        <v>1144680</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="2"/>
-        <v>1901640</v>
+        <v>1481640</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="2"/>
-        <v>1023430</v>
+        <v>798430</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="2"/>
-        <v>1710290</v>
+        <v>1335290</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="2"/>
-        <v>2460290</v>
+        <v>1897790</v>
       </c>
       <c r="J13" s="10">
         <f t="shared" si="2"/>
-        <v>3436790</v>
+        <v>2649290</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="2"/>
-        <v>1776740</v>
+        <v>1371740</v>
       </c>
       <c r="L13" s="10">
         <f t="shared" si="2"/>
-        <v>2948540</v>
+        <v>2273540</v>
       </c>
       <c r="M13" s="10">
         <f t="shared" si="2"/>
-        <v>2948540</v>
+        <v>2273540</v>
       </c>
       <c r="N13" s="10">
         <f t="shared" si="2"/>
-        <v>4118100</v>
+        <v>3173100</v>
       </c>
       <c r="O13" s="10">
         <f t="shared" si="2"/>
-        <v>25860140</v>
+        <v>20010140</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -3366,59 +3371,59 @@
       </c>
       <c r="B14" s="14">
         <f>(B7+B13)</f>
-        <v>11385903</v>
+        <v>8600258</v>
       </c>
       <c r="C14" s="14">
         <f t="shared" ref="C14:O14" si="3">(C7+C13)</f>
-        <v>12202043</v>
+        <v>9236398</v>
       </c>
       <c r="D14" s="14">
         <f t="shared" si="3"/>
-        <v>13233857.210000001</v>
+        <v>9992212.2100000009</v>
       </c>
       <c r="E14" s="14">
         <f t="shared" si="3"/>
-        <v>14483391.420000002</v>
+        <v>10917746.420000002</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="3"/>
-        <v>16165885.630000003</v>
+        <v>12180240.630000003</v>
       </c>
       <c r="G14" s="14">
         <f t="shared" si="3"/>
-        <v>16940169.840000004</v>
+        <v>12729524.840000004</v>
       </c>
       <c r="H14" s="14">
         <f t="shared" si="3"/>
-        <v>18431314.050000004</v>
+        <v>13845669.050000004</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="3"/>
-        <v>20672458.260000005</v>
+        <v>15524313.260000005</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="3"/>
-        <v>23890102.470000006</v>
+        <v>17954457.470000006</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="3"/>
-        <v>25417696.680000007</v>
+        <v>19077051.680000007</v>
       </c>
       <c r="L14" s="14">
         <f t="shared" si="3"/>
-        <v>28147090.890000008</v>
+        <v>21131445.890000008</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" si="3"/>
-        <v>30876485.100000009</v>
+        <v>23185840.100000009</v>
       </c>
       <c r="N14" s="14">
         <f t="shared" si="3"/>
-        <v>34775439.31000001</v>
+        <v>26139794.31000001</v>
       </c>
       <c r="O14" s="14">
         <f t="shared" si="3"/>
-        <v>25860140</v>
+        <v>20010140</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4833,59 +4838,59 @@
       </c>
       <c r="B45" s="14">
         <f>(B14-B44)</f>
-        <v>11385903</v>
+        <v>8600258</v>
       </c>
       <c r="C45" s="14">
         <f t="shared" ref="C45:O45" si="8">(C14-C44)</f>
-        <v>11982897.210000001</v>
+        <v>9017252.2100000009</v>
       </c>
       <c r="D45" s="14">
         <f t="shared" si="8"/>
-        <v>13014711.420000002</v>
+        <v>9773066.4200000018</v>
       </c>
       <c r="E45" s="14">
         <f t="shared" si="8"/>
-        <v>14264245.630000003</v>
+        <v>10698600.630000003</v>
       </c>
       <c r="F45" s="14">
         <f t="shared" si="8"/>
-        <v>15916739.840000004</v>
+        <v>11931094.840000004</v>
       </c>
       <c r="G45" s="14">
         <f t="shared" si="8"/>
-        <v>16721024.050000004</v>
+        <v>12510379.050000004</v>
       </c>
       <c r="H45" s="14">
         <f t="shared" si="8"/>
-        <v>18212168.260000005</v>
+        <v>13626523.260000005</v>
       </c>
       <c r="I45" s="14">
         <f t="shared" si="8"/>
-        <v>20453312.470000006</v>
+        <v>15305167.470000006</v>
       </c>
       <c r="J45" s="14">
         <f t="shared" si="8"/>
-        <v>23640956.680000007</v>
+        <v>17705311.680000007</v>
       </c>
       <c r="K45" s="14">
         <f t="shared" si="8"/>
-        <v>25198550.890000008</v>
+        <v>18857905.890000008</v>
       </c>
       <c r="L45" s="14">
         <f t="shared" si="8"/>
-        <v>27927945.100000009</v>
+        <v>20912300.100000009</v>
       </c>
       <c r="M45" s="14">
         <f t="shared" si="8"/>
-        <v>30657339.31000001</v>
+        <v>22966694.31000001</v>
       </c>
       <c r="N45" s="14">
         <f t="shared" si="8"/>
-        <v>34526293.520000011</v>
+        <v>25890648.520000011</v>
       </c>
       <c r="O45" s="14">
         <f t="shared" si="8"/>
-        <v>23140390.52</v>
+        <v>17290390.52</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -5048,8 +5053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5148,55 +5153,55 @@
         <v>2</v>
       </c>
       <c r="B7" s="14">
-        <v>34526294</v>
+        <v>25890648.520000011</v>
       </c>
       <c r="C7" s="33">
         <f>B45</f>
-        <v>34526294</v>
+        <v>25890648.520000011</v>
       </c>
       <c r="D7" s="33">
         <f t="shared" ref="D7:N7" si="1">C45</f>
-        <v>35566976</v>
+        <v>26661330.520000011</v>
       </c>
       <c r="E7" s="33">
         <f t="shared" si="1"/>
-        <v>37258958</v>
+        <v>27939312.520000011</v>
       </c>
       <c r="F7" s="33">
         <f t="shared" si="1"/>
-        <v>39276900</v>
+        <v>29471254.520000011</v>
       </c>
       <c r="G7" s="33">
         <f t="shared" si="1"/>
-        <v>41994882</v>
+        <v>31559236.520000011</v>
       </c>
       <c r="H7" s="33">
         <f t="shared" si="1"/>
-        <v>43648754</v>
+        <v>32808108.520000011</v>
       </c>
       <c r="I7" s="33">
         <f t="shared" si="1"/>
-        <v>46531686</v>
+        <v>35016040.520000011</v>
       </c>
       <c r="J7" s="33">
         <f t="shared" si="1"/>
-        <v>50764618</v>
+        <v>38236472.520000011</v>
       </c>
       <c r="K7" s="33">
         <f t="shared" si="1"/>
-        <v>56725250</v>
+        <v>42779604.520000011</v>
       </c>
       <c r="L7" s="33">
         <f t="shared" si="1"/>
-        <v>59493432</v>
+        <v>44872786.520000011</v>
       </c>
       <c r="M7" s="33">
         <f t="shared" si="1"/>
-        <v>64214614</v>
+        <v>48468968.520000011</v>
       </c>
       <c r="N7" s="33">
         <f t="shared" si="1"/>
-        <v>68935796</v>
+        <v>52065150.520000011</v>
       </c>
       <c r="O7" s="33"/>
     </row>
@@ -5245,44 +5250,44 @@
         <v>0</v>
       </c>
       <c r="C10" s="12">
-        <v>1223280</v>
+        <v>953280</v>
       </c>
       <c r="D10" s="12">
-        <v>1874580</v>
+        <v>1460580</v>
       </c>
       <c r="E10" s="12">
-        <v>2200540</v>
+        <v>1714540</v>
       </c>
       <c r="F10" s="12">
-        <v>2930580</v>
+        <v>2300580</v>
       </c>
       <c r="G10" s="12">
-        <v>1836470</v>
+        <v>1431470</v>
       </c>
       <c r="H10" s="12">
-        <v>3065530</v>
+        <v>2390530</v>
       </c>
       <c r="I10" s="12">
-        <v>4415530</v>
+        <v>3403030</v>
       </c>
       <c r="J10" s="12">
-        <v>6173230</v>
+        <v>4755730</v>
       </c>
       <c r="K10" s="12">
-        <v>2950780</v>
+        <v>2275780</v>
       </c>
       <c r="L10" s="12">
-        <v>4903780</v>
+        <v>3778780</v>
       </c>
       <c r="M10" s="12">
-        <v>4903780</v>
+        <v>3778780</v>
       </c>
       <c r="N10" s="12">
-        <v>6854540</v>
+        <v>5279540</v>
       </c>
       <c r="O10" s="12">
         <f>SUM(C10:N10)</f>
-        <v>43332620</v>
+        <v>33522620</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -5391,55 +5396,55 @@
       </c>
       <c r="C13" s="10">
         <f t="shared" ref="C13:O13" si="3">SUM(C10:C12)</f>
-        <v>1223280</v>
+        <v>953280</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="3"/>
-        <v>1874580</v>
+        <v>1460580</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="3"/>
-        <v>2200540</v>
+        <v>1714540</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="3"/>
-        <v>2930580</v>
+        <v>2300580</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="3"/>
-        <v>1836470</v>
+        <v>1431470</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="3"/>
-        <v>3065530</v>
+        <v>2390530</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="3"/>
-        <v>4415530</v>
+        <v>3403030</v>
       </c>
       <c r="J13" s="10">
         <f t="shared" si="3"/>
-        <v>6173230</v>
+        <v>4755730</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="3"/>
-        <v>2950780</v>
+        <v>2275780</v>
       </c>
       <c r="L13" s="10">
         <f t="shared" si="3"/>
-        <v>4903780</v>
+        <v>3778780</v>
       </c>
       <c r="M13" s="10">
         <f t="shared" si="3"/>
-        <v>4903780</v>
+        <v>3778780</v>
       </c>
       <c r="N13" s="10">
         <f t="shared" si="3"/>
-        <v>6854540</v>
+        <v>5279540</v>
       </c>
       <c r="O13" s="10">
         <f t="shared" si="3"/>
-        <v>43332620</v>
+        <v>33522620</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -5448,59 +5453,59 @@
       </c>
       <c r="B14" s="14">
         <f>(B7+B13)</f>
-        <v>34526294</v>
+        <v>25890648.520000011</v>
       </c>
       <c r="C14" s="14">
         <f t="shared" ref="C14:O14" si="4">(C7+C13)</f>
-        <v>35749574</v>
+        <v>26843928.520000011</v>
       </c>
       <c r="D14" s="14">
         <f t="shared" si="4"/>
-        <v>37441556</v>
+        <v>28121910.520000011</v>
       </c>
       <c r="E14" s="14">
         <f t="shared" si="4"/>
-        <v>39459498</v>
+        <v>29653852.520000011</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="4"/>
-        <v>42207480</v>
+        <v>31771834.520000011</v>
       </c>
       <c r="G14" s="14">
         <f t="shared" si="4"/>
-        <v>43831352</v>
+        <v>32990706.520000011</v>
       </c>
       <c r="H14" s="14">
         <f t="shared" si="4"/>
-        <v>46714284</v>
+        <v>35198638.520000011</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="4"/>
-        <v>50947216</v>
+        <v>38419070.520000011</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="4"/>
-        <v>56937848</v>
+        <v>42992202.520000011</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="4"/>
-        <v>59676030</v>
+        <v>45055384.520000011</v>
       </c>
       <c r="L14" s="14">
         <f t="shared" si="4"/>
-        <v>64397212</v>
+        <v>48651566.520000011</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" si="4"/>
-        <v>69118394</v>
+        <v>52247748.520000011</v>
       </c>
       <c r="N14" s="14">
         <f t="shared" si="4"/>
-        <v>75790336</v>
+        <v>57344690.520000011</v>
       </c>
       <c r="O14" s="14">
         <f t="shared" si="4"/>
-        <v>43332620</v>
+        <v>33522620</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -6875,59 +6880,59 @@
       </c>
       <c r="B45" s="14">
         <f>(B14-B44)</f>
-        <v>34526294</v>
+        <v>25890648.520000011</v>
       </c>
       <c r="C45" s="14">
         <f t="shared" ref="C45:O45" si="6">(C14-C44)</f>
-        <v>35566976</v>
+        <v>26661330.520000011</v>
       </c>
       <c r="D45" s="14">
         <f t="shared" si="6"/>
-        <v>37258958</v>
+        <v>27939312.520000011</v>
       </c>
       <c r="E45" s="14">
         <f t="shared" si="6"/>
-        <v>39276900</v>
+        <v>29471254.520000011</v>
       </c>
       <c r="F45" s="14">
         <f t="shared" si="6"/>
-        <v>41994882</v>
+        <v>31559236.520000011</v>
       </c>
       <c r="G45" s="14">
         <f t="shared" si="6"/>
-        <v>43648754</v>
+        <v>32808108.520000011</v>
       </c>
       <c r="H45" s="14">
         <f t="shared" si="6"/>
-        <v>46531686</v>
+        <v>35016040.520000011</v>
       </c>
       <c r="I45" s="14">
         <f t="shared" si="6"/>
-        <v>50764618</v>
+        <v>38236472.520000011</v>
       </c>
       <c r="J45" s="14">
         <f t="shared" si="6"/>
-        <v>56725250</v>
+        <v>42779604.520000011</v>
       </c>
       <c r="K45" s="14">
         <f t="shared" si="6"/>
-        <v>59493432</v>
+        <v>44872786.520000011</v>
       </c>
       <c r="L45" s="14">
         <f t="shared" si="6"/>
-        <v>64214614</v>
+        <v>48468968.520000011</v>
       </c>
       <c r="M45" s="14">
         <f t="shared" si="6"/>
-        <v>68935796</v>
+        <v>52065150.520000011</v>
       </c>
       <c r="N45" s="14">
         <f t="shared" si="6"/>
-        <v>75577738</v>
+        <v>57132092.520000011</v>
       </c>
       <c r="O45" s="14">
         <f t="shared" si="6"/>
-        <v>40612870.520000003</v>
+        <v>30802870.52</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -7090,8 +7095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -7192,55 +7197,55 @@
         <v>2</v>
       </c>
       <c r="B7" s="33">
-        <v>75577738</v>
+        <v>57132092.520000011</v>
       </c>
       <c r="C7" s="33">
         <f>B45</f>
-        <v>75577738</v>
+        <v>57132092.520000011</v>
       </c>
       <c r="D7" s="33">
         <f t="shared" ref="D7:N7" si="1">C45</f>
-        <v>77431460</v>
+        <v>58535814.520000011</v>
       </c>
       <c r="E7" s="33">
         <f t="shared" si="1"/>
-        <v>80369442</v>
+        <v>60783796.520000011</v>
       </c>
       <c r="F7" s="33">
         <f t="shared" si="1"/>
-        <v>83849864</v>
+        <v>63454218.520000011</v>
       </c>
       <c r="G7" s="33">
         <f t="shared" si="1"/>
-        <v>88382686</v>
+        <v>66937040.520000011</v>
       </c>
       <c r="H7" s="33">
         <f t="shared" si="1"/>
-        <v>90748123</v>
+        <v>68739977.520000011</v>
       </c>
       <c r="I7" s="33">
         <f t="shared" si="1"/>
-        <v>94817170</v>
+        <v>71871524.520000011</v>
       </c>
       <c r="J7" s="33">
         <f t="shared" si="1"/>
-        <v>100761217</v>
+        <v>76409321.520000011</v>
       </c>
       <c r="K7" s="33">
         <f t="shared" si="1"/>
-        <v>109116514</v>
+        <v>82795868.520000011</v>
       </c>
       <c r="L7" s="33">
         <f t="shared" si="1"/>
-        <v>112912261</v>
+        <v>85680365.520000011</v>
       </c>
       <c r="M7" s="33">
         <f t="shared" si="1"/>
-        <v>119344558</v>
+        <v>90593912.520000011</v>
       </c>
       <c r="N7" s="33">
         <f t="shared" si="1"/>
-        <v>125776855</v>
+        <v>95507459.520000011</v>
       </c>
       <c r="O7" s="33"/>
     </row>
@@ -7289,44 +7294,44 @@
         <v>0</v>
       </c>
       <c r="C10" s="12">
-        <v>2036320</v>
+        <v>1586320</v>
       </c>
       <c r="D10" s="12">
-        <v>3120580</v>
+        <v>2430580</v>
       </c>
       <c r="E10" s="12">
-        <v>3663020</v>
+        <v>2853020</v>
       </c>
       <c r="F10" s="12">
-        <v>4745420</v>
+        <v>3695420</v>
       </c>
       <c r="G10" s="12">
-        <v>2548035</v>
+        <v>1985535</v>
       </c>
       <c r="H10" s="12">
-        <v>4251645</v>
+        <v>3314145</v>
       </c>
       <c r="I10" s="12">
-        <v>6126645</v>
+        <v>4720395</v>
       </c>
       <c r="J10" s="12">
-        <v>8567895</v>
+        <v>6599145</v>
       </c>
       <c r="K10" s="12">
-        <v>3978345</v>
+        <v>3067095</v>
       </c>
       <c r="L10" s="12">
-        <v>6614895</v>
+        <v>5096145</v>
       </c>
       <c r="M10" s="12">
-        <v>6614895</v>
+        <v>5096145</v>
       </c>
       <c r="N10" s="12">
-        <v>9249204.9999999981</v>
+        <v>7122954.9999999991</v>
       </c>
       <c r="O10" s="10">
         <f>SUM(C10:N10)</f>
-        <v>61516900</v>
+        <v>47566900</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -7435,55 +7440,55 @@
       </c>
       <c r="C13" s="10">
         <f t="shared" ref="C13:N13" si="2">SUM(C10:C12)</f>
-        <v>2036320</v>
+        <v>1586320</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="2"/>
-        <v>3120580</v>
+        <v>2430580</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="2"/>
-        <v>3663020</v>
+        <v>2853020</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="2"/>
-        <v>4745420</v>
+        <v>3695420</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="2"/>
-        <v>2548035</v>
+        <v>1985535</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="2"/>
-        <v>4251645</v>
+        <v>3314145</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="2"/>
-        <v>6126645</v>
+        <v>4720395</v>
       </c>
       <c r="J13" s="10">
         <f t="shared" si="2"/>
-        <v>8567895</v>
+        <v>6599145</v>
       </c>
       <c r="K13" s="10">
         <f t="shared" si="2"/>
-        <v>3978345</v>
+        <v>3067095</v>
       </c>
       <c r="L13" s="10">
         <f t="shared" si="2"/>
-        <v>6614895</v>
+        <v>5096145</v>
       </c>
       <c r="M13" s="10">
         <f t="shared" si="2"/>
-        <v>6614895</v>
+        <v>5096145</v>
       </c>
       <c r="N13" s="10">
         <f t="shared" si="2"/>
-        <v>9249204.9999999981</v>
+        <v>7122954.9999999991</v>
       </c>
       <c r="O13" s="10">
         <f>SUM(C13:N13)</f>
-        <v>61516900</v>
+        <v>47566900</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
@@ -7492,59 +7497,59 @@
       </c>
       <c r="B14" s="14">
         <f>(B7+B13)</f>
-        <v>75577738</v>
+        <v>57132092.520000011</v>
       </c>
       <c r="C14" s="14">
         <f t="shared" ref="C14:O14" si="3">(C7+C13)</f>
-        <v>77614058</v>
+        <v>58718412.520000011</v>
       </c>
       <c r="D14" s="14">
         <f t="shared" si="3"/>
-        <v>80552040</v>
+        <v>60966394.520000011</v>
       </c>
       <c r="E14" s="14">
         <f t="shared" si="3"/>
-        <v>84032462</v>
+        <v>63636816.520000011</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="3"/>
-        <v>88595284</v>
+        <v>67149638.520000011</v>
       </c>
       <c r="G14" s="14">
         <f t="shared" si="3"/>
-        <v>90930721</v>
+        <v>68922575.520000011</v>
       </c>
       <c r="H14" s="14">
         <f t="shared" si="3"/>
-        <v>94999768</v>
+        <v>72054122.520000011</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="3"/>
-        <v>100943815</v>
+        <v>76591919.520000011</v>
       </c>
       <c r="J14" s="14">
         <f t="shared" si="3"/>
-        <v>109329112</v>
+        <v>83008466.520000011</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="3"/>
-        <v>113094859</v>
+        <v>85862963.520000011</v>
       </c>
       <c r="L14" s="14">
         <f t="shared" si="3"/>
-        <v>119527156</v>
+        <v>90776510.520000011</v>
       </c>
       <c r="M14" s="14">
         <f t="shared" si="3"/>
-        <v>125959453</v>
+        <v>95690057.520000011</v>
       </c>
       <c r="N14" s="14">
         <f t="shared" si="3"/>
-        <v>135026060</v>
+        <v>102630414.52000001</v>
       </c>
       <c r="O14" s="14">
         <f t="shared" si="3"/>
-        <v>61516900</v>
+        <v>47566900</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -8919,59 +8924,59 @@
       </c>
       <c r="B45" s="14">
         <f>(B14-B44)</f>
-        <v>75577738</v>
+        <v>57132092.520000011</v>
       </c>
       <c r="C45" s="14">
         <f t="shared" ref="C45:O45" si="5">(C14-C44)</f>
-        <v>77431460</v>
+        <v>58535814.520000011</v>
       </c>
       <c r="D45" s="14">
         <f t="shared" si="5"/>
-        <v>80369442</v>
+        <v>60783796.520000011</v>
       </c>
       <c r="E45" s="14">
         <f t="shared" si="5"/>
-        <v>83849864</v>
+        <v>63454218.520000011</v>
       </c>
       <c r="F45" s="14">
         <f t="shared" si="5"/>
-        <v>88382686</v>
+        <v>66937040.520000011</v>
       </c>
       <c r="G45" s="14">
         <f t="shared" si="5"/>
-        <v>90748123</v>
+        <v>68739977.520000011</v>
       </c>
       <c r="H45" s="14">
         <f t="shared" si="5"/>
-        <v>94817170</v>
+        <v>71871524.520000011</v>
       </c>
       <c r="I45" s="14">
         <f t="shared" si="5"/>
-        <v>100761217</v>
+        <v>76409321.520000011</v>
       </c>
       <c r="J45" s="14">
         <f t="shared" si="5"/>
-        <v>109116514</v>
+        <v>82795868.520000011</v>
       </c>
       <c r="K45" s="14">
         <f t="shared" si="5"/>
-        <v>112912261</v>
+        <v>85680365.520000011</v>
       </c>
       <c r="L45" s="14">
         <f t="shared" si="5"/>
-        <v>119344558</v>
+        <v>90593912.520000011</v>
       </c>
       <c r="M45" s="14">
         <f t="shared" si="5"/>
-        <v>125776855</v>
+        <v>95507459.520000011</v>
       </c>
       <c r="N45" s="14">
         <f t="shared" si="5"/>
-        <v>134813462</v>
+        <v>102417816.52000001</v>
       </c>
       <c r="O45" s="14">
         <f t="shared" si="5"/>
-        <v>58797150.520000003</v>
+        <v>44847150.520000003</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>